<commit_message>
ML_PL ANN testing finished
</commit_message>
<xml_diff>
--- a/ML_PL_new/realbet.xlsx
+++ b/ML_PL_new/realbet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\.Data files\TSDP\ML_PL_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\..Data\TSDP\ML_PL_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98479FBF-F47F-4138-8824-A19729EF1557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="0" windowWidth="7160" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12045" yWindow="0" windowWidth="7155" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
   </numFmts>
@@ -109,7 +108,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1747,24 +1746,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H15" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" customWidth="1"/>
-    <col min="11" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>Date</v>
@@ -1811,7 +1810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45743.875</v>
@@ -1858,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45744.84375</v>
@@ -1905,7 +1904,7 @@
         <v>939.58668912417102</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45744.854166666657</v>
@@ -1952,7 +1951,7 @@
         <v>52.439940595617699</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45744.864583333343</v>
@@ -1999,7 +1998,7 @@
         <v>160.42348255147064</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45744.875</v>
@@ -2046,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.583333333343</v>
@@ -2093,7 +2092,7 @@
         <v>0.68606633912098558</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.625</v>
@@ -2140,7 +2139,7 @@
         <v>72.587816557279737</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.625</v>
@@ -2187,7 +2186,7 @@
         <v>378.18927968865364</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.645833333343</v>
@@ -2234,7 +2233,7 @@
         <v>201.76325531107847</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.645833333343</v>
@@ -2281,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.645833333343</v>
@@ -2328,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.645833333343</v>
@@ -2375,7 +2374,7 @@
         <v>259.25034887473305</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.645833333343</v>
@@ -2422,7 +2421,7 @@
         <v>369.22215190610979</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.645833333343</v>
@@ -2469,7 +2468,7 @@
         <v>62.332626694519362</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.677083333343</v>
@@ -2516,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.6875</v>
@@ -2563,7 +2562,7 @@
         <v>52.860927634856672</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.708333333343</v>
@@ -2610,7 +2609,7 @@
         <v>697.47437858270666</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.75</v>
@@ -2657,7 +2656,7 @@
         <v>907.16690583300897</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.75</v>
@@ -2703,12 +2702,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N20" s="1">
-        <f>SUM(J16:L59)</f>
-        <v>2867.4425730471444</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.770833333343</v>
@@ -2755,7 +2750,7 @@
         <v>130.22289255810836</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.770833333343</v>
@@ -2802,7 +2797,7 @@
         <v>207.16062735407209</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.78125</v>
@@ -2849,7 +2844,7 @@
         <v>210.23883989710109</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.78125</v>
@@ -2896,7 +2891,7 @@
         <v>16.003161656843357</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.791666666657</v>
@@ -2922,31 +2917,28 @@
         <v>0.99276296976950928</v>
       </c>
       <c r="G25">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="H25">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="I25">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L25" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1.18</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="3"/>
+        <v>1153.2170051655969</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.854166666657</v>
@@ -2972,31 +2964,28 @@
         <v>0.62024221792854128</v>
       </c>
       <c r="G26">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>1.67</v>
       </c>
       <c r="H26">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>3.85</v>
       </c>
       <c r="I26">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L26" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="3"/>
+        <v>150.08650640305044</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.864583333343</v>
@@ -3022,31 +3011,28 @@
         <v>0.9072014918342296</v>
       </c>
       <c r="G27">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H27">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>3.55</v>
       </c>
       <c r="I27">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K27" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L27" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1.79</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="3"/>
+        <v>630.27535977782031</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.875</v>
@@ -3072,31 +3058,28 @@
         <v>0.77552082589659643</v>
       </c>
       <c r="G28">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H28">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>3.65</v>
       </c>
       <c r="I28">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K28" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+        <v>3.45</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="3"/>
+        <v>283.18702824071619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.875</v>
@@ -3122,31 +3105,28 @@
         <v>0.76151137402271829</v>
       </c>
       <c r="G29">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="H29">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>3.55</v>
       </c>
       <c r="I29">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K29" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1.95</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="3"/>
+        <v>373.97121985294046</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.875</v>
@@ -3172,31 +3152,19 @@
         <v>2.7965535538507029E-3</v>
       </c>
       <c r="G30">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="H30">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>7.75</v>
       </c>
       <c r="I30">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K30" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L30" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45745.878472222219</v>
@@ -3222,31 +3190,23 @@
         <v>6.262615804121906E-6</v>
       </c>
       <c r="G31">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>1.99</v>
       </c>
       <c r="H31">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I31">
-        <f>[1]Sheet1!$A$1:$I$59</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K31" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L31" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+        <v>3.85</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="N31" s="1">
+        <f>SUM(J26:L59)</f>
+        <v>1437.5201142745275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.510416666657</v>
@@ -3296,7 +3256,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.520833333343</v>
@@ -3346,7 +3306,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.583333333343</v>
@@ -3396,7 +3356,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.604166666657</v>
@@ -3446,7 +3406,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.604166666657</v>
@@ -3496,7 +3456,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.604166666657</v>
@@ -3546,7 +3506,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.625</v>
@@ -3596,7 +3556,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.625</v>
@@ -3646,7 +3606,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.645833333343</v>
@@ -3696,7 +3656,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.645833333343</v>
@@ -3746,7 +3706,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.677083333343</v>
@@ -3796,7 +3756,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.697916666657</v>
@@ -3846,7 +3806,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.71875</v>
@@ -3896,7 +3856,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.71875</v>
@@ -3946,7 +3906,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.71875</v>
@@ -3996,7 +3956,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.729166666657</v>
@@ -4046,7 +4006,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.75</v>
@@ -4096,7 +4056,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.75</v>
@@ -4146,7 +4106,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.770833333343</v>
@@ -4196,7 +4156,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.854166666657</v>
@@ -4246,7 +4206,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.864583333343</v>
@@ -4296,7 +4256,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.864583333343</v>
@@ -4346,7 +4306,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45746.875</v>
@@ -4396,7 +4356,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45747.770833333343</v>
@@ -4446,7 +4406,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45747.864583333343</v>
@@ -4496,7 +4456,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45747.875</v>
@@ -4546,7 +4506,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45748.822916666657</v>
@@ -4596,7 +4556,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <f>[1]Sheet1!$A$1:$I$59</f>
         <v>45748.833333333343</v>

</xml_diff>